<commit_message>
update busy marks - button=I AM NOT IN AUD
</commit_message>
<xml_diff>
--- a/backend/backend/start_data.xlsx
+++ b/backend/backend/start_data.xlsx
@@ -18,7 +18,9 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b val="true"/>
+        <sz val="11"/>
       </rPr>
       <t>Название</t>
     </r>
@@ -26,7 +28,9 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b val="true"/>
+        <sz val="11"/>
       </rPr>
       <t>Описание</t>
     </r>
@@ -52,8 +56,10 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b val="true"/>
         <color rgb="000000" tint="0"/>
+        <sz val="11"/>
       </rPr>
       <t>Название ВУЗа</t>
     </r>
@@ -61,8 +67,10 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b val="true"/>
         <color rgb="000000" tint="0"/>
+        <sz val="11"/>
       </rPr>
       <t>Название здания</t>
     </r>
@@ -70,8 +78,10 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b val="true"/>
         <color rgb="000000" tint="0"/>
+        <sz val="11"/>
       </rPr>
       <t>Описание</t>
     </r>
@@ -156,6 +166,30 @@
   </si>
   <si>
     <t>Аудитория отсутствует для бронирования</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto"/>
+        <b val="false"/>
+        <i val="false"/>
+        <color rgb="333333" tint="0"/>
+        <sz val="9.80000019073486"/>
+      </rPr>
+      <t>Резерв</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto"/>
+        <b val="false"/>
+        <i val="false"/>
+        <color rgb="333333" tint="0"/>
+        <sz val="9.80000019073486"/>
+      </rPr>
+      <t>Аудитория находиться в резерве у сервиса бронирования</t>
+    </r>
   </si>
   <si>
     <t>Название ВУЗа</t>
@@ -341,7 +375,7 @@
   <numFmts>
     <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <color theme="1" tint="0"/>
@@ -353,11 +387,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="true"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="true"/>
       <color rgb="000000" tint="0"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="true"/>
@@ -376,8 +414,15 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="false"/>
+      <i val="false"/>
+      <color rgb="333333" tint="0"/>
+      <sz val="9.80000019073486"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +432,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="F2F2F2" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF" tint="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -402,15 +452,18 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false"/>
-    <xf applyFill="true" borderId="0" fillId="2" fontId="0" quotePrefix="false"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="0" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="2" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="3" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="4" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="5" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="6" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
+    <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="3" fontId="7" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -852,6 +905,14 @@
         <v>30</v>
       </c>
     </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.590555548667908" footer="0.5" header="0.5" left="0.590555548667908" right="0.590555548667908" top="0.590555548667908"/>
   <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297.1798mm" paperSize="9" paperWidth="210.0438mm" scale="100"/>
@@ -879,22 +940,22 @@
   <sheetData>
     <row customFormat="true" ht="15" outlineLevel="0" r="1" s="2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="2">
@@ -908,7 +969,7 @@
         <v>510</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>25</v>
@@ -929,7 +990,7 @@
         <v>511</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>27</v>
@@ -950,7 +1011,7 @@
         <v>512</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>23</v>
@@ -971,7 +1032,7 @@
         <v>513</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>29</v>
@@ -992,7 +1053,7 @@
         <v>514</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>23</v>
@@ -1013,7 +1074,7 @@
         <v>515</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>23</v>
@@ -1034,7 +1095,7 @@
         <v>516</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>25</v>
@@ -1055,7 +1116,7 @@
         <v>517</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>27</v>
@@ -1075,7 +1136,7 @@
         <v>411</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>23</v>
@@ -1096,7 +1157,7 @@
         <v>412</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>29</v>
@@ -1117,7 +1178,7 @@
         <v>413</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>27</v>
@@ -1138,7 +1199,7 @@
         <v>414</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>23</v>
@@ -1158,7 +1219,7 @@
         <v>425</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>25</v>
@@ -1178,7 +1239,7 @@
         <v>423</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>23</v>
@@ -1198,7 +1259,7 @@
         <v>422</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>29</v>
@@ -1230,21 +1291,21 @@
   <sheetData>
     <row customFormat="true" ht="15" outlineLevel="0" r="1" s="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>28</v>

</xml_diff>